<commit_message>
CV Reporte de ventas, facturas emitidas y recibos emitidos
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacEmitidas.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacEmitidas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8540CD2C-ECFD-D64A-ADED-1E4DE8AFAF08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BCF8AF-7598-7640-80D9-17852366DA3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="7580" windowWidth="35960" windowHeight="18240" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>% IVA</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>CANTIDAD</t>
+  </si>
+  <si>
+    <t>TOT SIN IMPU</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32A76B9-2613-7147-BFF0-D21843D4C7F8}">
-  <dimension ref="A2:O10"/>
+  <dimension ref="A2:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,13 +516,14 @@
     <col min="4" max="6" width="22.5" customWidth="1"/>
     <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.5" customWidth="1"/>
-    <col min="12" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.5" customWidth="1"/>
+    <col min="13" max="14" width="13.5" customWidth="1"/>
+    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -537,8 +541,9 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -549,7 +554,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -560,7 +565,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -571,7 +576,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -582,7 +587,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -593,7 +598,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -622,27 +627,30 @@
         <v>14</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="P10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A2:P2"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B8:D8"/>

</xml_diff>

<commit_message>
CV pantalla facturas emitidas, popup de pagos, nuefo formato de exportación
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacEmitidas.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacEmitidas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BCF8AF-7598-7640-80D9-17852366DA3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0544DDA6-09CE-9948-AA9C-2D7EB6D2AB1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="7580" windowWidth="35960" windowHeight="18240" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
+    <workbookView xWindow="1520" yWindow="7580" windowWidth="42320" windowHeight="20280" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>% IVA</t>
   </si>
@@ -63,9 +63,6 @@
     <t>ESTADO</t>
   </si>
   <si>
-    <t>AUT S.R.I.</t>
-  </si>
-  <si>
     <t>SUBTOTAL</t>
   </si>
   <si>
@@ -81,16 +78,25 @@
     <t>PAGO</t>
   </si>
   <si>
-    <t>ENTREGA</t>
-  </si>
-  <si>
-    <t>CAMBIO</t>
-  </si>
-  <si>
     <t>CANTIDAD</t>
   </si>
   <si>
     <t>TOT SIN IMPU</t>
+  </si>
+  <si>
+    <t>RUC</t>
+  </si>
+  <si>
+    <t>RETENCIÓN</t>
+  </si>
+  <si>
+    <t>A PAGAR</t>
+  </si>
+  <si>
+    <t>GUÍA REMISIÓN</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
   </si>
 </sst>
 </file>
@@ -170,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -179,6 +185,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,103 +511,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32A76B9-2613-7147-BFF0-D21843D4C7F8}">
-  <dimension ref="A2:P10"/>
+  <dimension ref="A2:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.6640625" customWidth="1"/>
-    <col min="4" max="6" width="22.5" customWidth="1"/>
-    <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.5" customWidth="1"/>
-    <col min="13" max="14" width="13.5" customWidth="1"/>
-    <col min="15" max="15" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="2" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.5" customWidth="1"/>
+    <col min="15" max="16" width="13.5" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -606,56 +629,62 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="K10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="Q10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="R10" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A2:P2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="A2:R2"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CV arreglo de reportes en los comprobantes electrónicos
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacEmitidas.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-FacEmitidas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0544DDA6-09CE-9948-AA9C-2D7EB6D2AB1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4FC678-4B54-9D44-9723-23A74FB97597}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="7580" windowWidth="42320" windowHeight="20280" xr2:uid="{E9788733-D204-D84A-A824-443E01B2DF94}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
-    <t>% IVA</t>
-  </si>
-  <si>
     <t>ESTABLECIMEINTO :</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>DESCUENTO</t>
   </si>
   <si>
-    <t>%ICE</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -97,6 +91,12 @@
   </si>
   <si>
     <t>EMAIL</t>
+  </si>
+  <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>ICE</t>
   </si>
 </sst>
 </file>
@@ -514,7 +514,7 @@
   <dimension ref="A2:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,7 +536,7 @@
   <sheetData>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -558,7 +558,7 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -571,7 +571,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -584,7 +584,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -597,7 +597,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -610,7 +610,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -623,58 +623,58 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="s">
+      <c r="R10" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>